<commit_message>
updated Timecard; load csv added to main
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/Ansari_TimeCard.xlsx
+++ b/YellowLib/YellowLib/Ansari_TimeCard.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="20">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -641,8 +641,8 @@
   </sheetPr>
   <dimension ref="B1:H39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -716,15 +716,15 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>35.75</v>
+        <v>40.75</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
-        <v>35.75</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1118,11 +1118,11 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>11</v>
+      <c r="B26" s="4">
+        <v>43573</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.41666666666666669</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>12</v>
@@ -1130,20 +1130,20 @@
       <c r="E26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>14</v>
+      <c r="F26" s="6">
+        <v>0.45833333333333331</v>
       </c>
       <c r="G26" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>0.99999999999999911</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>11</v>
+      <c r="B27" s="4">
+        <v>43576</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.58333333333333337</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>12</v>
@@ -1151,20 +1151,20 @@
       <c r="E27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>14</v>
+      <c r="F27" s="6">
+        <v>0.66666666666666663</v>
       </c>
       <c r="G27" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>1.9999999999999982</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>11</v>
+      <c r="B28" s="4">
+        <v>43578</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.75</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>12</v>
@@ -1172,12 +1172,12 @@
       <c r="E28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>14</v>
+      <c r="F28" s="6">
+        <v>0.83333333333333337</v>
       </c>
       <c r="G28" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2.0000000000000009</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>